<commit_message>
open sourcing on github
</commit_message>
<xml_diff>
--- a/reference/Client A.xlsx
+++ b/reference/Client A.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="3060" windowWidth="18720" windowHeight="22900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="9160" yWindow="4140" windowWidth="29720" windowHeight="22900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="January Projects" sheetId="5" r:id="rId1"/>
@@ -92,6 +92,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$$-409]\ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="[$$-2409]\ #,##0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -131,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -139,6 +144,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,13 +504,13 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="8">
         <v>111</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="8">
         <v>112</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
         <v>113</v>
       </c>
     </row>
@@ -509,13 +518,13 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>15</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>1</v>
       </c>
     </row>
@@ -523,15 +532,15 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="7">
         <f>SUM(85*B3)</f>
         <v>425</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="7">
         <f t="shared" ref="C4:D4" si="0">SUM(85*C3)</f>
         <v>1275</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
@@ -540,13 +549,13 @@
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>12</v>
       </c>
     </row>
@@ -554,15 +563,15 @@
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="7">
         <f>SUM(55*B5)</f>
         <v>220</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <f t="shared" ref="C6:D6" si="1">SUM(55*C5)</f>
         <v>440</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <f t="shared" si="1"/>
         <v>660</v>
       </c>
@@ -571,15 +580,15 @@
       <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="7">
         <f>SUM(0.08*B8)</f>
         <v>51.6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="7">
         <f t="shared" ref="C7:D7" si="2">SUM(0.08*C8)</f>
         <v>137.20000000000002</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="7">
         <f t="shared" si="2"/>
         <v>59.6</v>
       </c>
@@ -588,15 +597,15 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="7">
         <f>SUM(B4+B6)</f>
         <v>645</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="7">
         <f t="shared" ref="C8:D8" si="3">SUM(C4+C6)</f>
         <v>1715</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <f t="shared" si="3"/>
         <v>745</v>
       </c>
@@ -605,15 +614,15 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="7">
         <f>SUM(B8+B7)</f>
         <v>696.6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="7">
         <f t="shared" ref="C9:D9" si="4">SUM(C8+C7)</f>
         <v>1852.2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="7">
         <f t="shared" si="4"/>
         <v>804.6</v>
       </c>
@@ -623,16 +632,13 @@
         <v>18</v>
       </c>
       <c r="B10" s="4">
-        <f ca="1">TODAY()</f>
-        <v>42682</v>
+        <v>42380</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" ref="C10:D10" ca="1" si="5">TODAY()</f>
-        <v>42682</v>
+        <v>42381</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>42682</v>
+        <v>42382</v>
       </c>
     </row>
   </sheetData>
@@ -644,15 +650,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="10.83203125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -665,13 +671,13 @@
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="6">
         <v>114</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="6">
         <v>115</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="6">
         <v>116</v>
       </c>
     </row>
@@ -679,13 +685,13 @@
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="6">
         <v>32</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>15</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="6">
         <v>27</v>
       </c>
     </row>
@@ -693,15 +699,15 @@
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <f>SUM(85*B3)</f>
         <v>2720</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="5">
         <f t="shared" ref="C4:D4" si="0">SUM(85*C3)</f>
         <v>1275</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="5">
         <f t="shared" si="0"/>
         <v>2295</v>
       </c>
@@ -710,13 +716,13 @@
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="6">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="6">
         <v>3</v>
       </c>
     </row>
@@ -724,15 +730,15 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <f>SUM(55*B5)</f>
         <v>220</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="5">
         <f t="shared" ref="C6:D6" si="1">SUM(55*C5)</f>
         <v>110</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <f t="shared" si="1"/>
         <v>165</v>
       </c>
@@ -741,15 +747,15 @@
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <f>SUM(0.08*B8)</f>
         <v>235.20000000000002</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="5">
         <f t="shared" ref="C7:D7" si="2">SUM(0.08*C8)</f>
         <v>110.8</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="5">
         <f t="shared" si="2"/>
         <v>196.8</v>
       </c>
@@ -758,15 +764,15 @@
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <f>SUM(B4+B6)</f>
         <v>2940</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="5">
         <f t="shared" ref="C8:D8" si="3">SUM(C4+C6)</f>
         <v>1385</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="5">
         <f t="shared" si="3"/>
         <v>2460</v>
       </c>
@@ -775,15 +781,15 @@
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <f>SUM(B8+B7)</f>
         <v>3175.2</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <f t="shared" ref="C9:D9" si="4">SUM(C8+C7)</f>
         <v>1495.8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <f t="shared" si="4"/>
         <v>2656.8</v>
       </c>
@@ -793,16 +799,13 @@
         <v>18</v>
       </c>
       <c r="B10" s="4">
-        <f ca="1">TODAY()</f>
-        <v>42682</v>
+        <v>42411</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" ref="C10:D10" ca="1" si="5">TODAY()</f>
-        <v>42682</v>
+        <v>42412</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" ca="1" si="5"/>
-        <v>42682</v>
+        <v>42413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>